<commit_message>
Atualizando planilha modelo para importação de militares.
</commit_message>
<xml_diff>
--- a/apis/src/main/resources/samples/modelo_importacao_militares.xlsx
+++ b/apis/src/main/resources/samples/modelo_importacao_militares.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">C.O.V.</t>
   </si>
   <si>
-    <t xml:space="preserve">REG874</t>
+    <t xml:space="preserve">REG00001</t>
   </si>
   <si>
     <t xml:space="preserve">TEN</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">NÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG532</t>
+    <t xml:space="preserve">REG00002</t>
   </si>
   <si>
     <t xml:space="preserve">SGT</t>
@@ -70,25 +70,25 @@
     <t xml:space="preserve">SIM</t>
   </si>
   <si>
-    <t xml:space="preserve">REG687</t>
+    <t xml:space="preserve">REG00003</t>
   </si>
   <si>
     <t xml:space="preserve">JOÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG920</t>
+    <t xml:space="preserve">REG00004</t>
   </si>
   <si>
     <t xml:space="preserve">PAULO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG385</t>
+    <t xml:space="preserve">REG00005</t>
   </si>
   <si>
     <t xml:space="preserve">MARIANA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG741</t>
+    <t xml:space="preserve">REG00006</t>
   </si>
   <si>
     <t xml:space="preserve">CB</t>
@@ -97,115 +97,115 @@
     <t xml:space="preserve">RAFAEL</t>
   </si>
   <si>
-    <t xml:space="preserve">REG829</t>
+    <t xml:space="preserve">REG00007</t>
   </si>
   <si>
     <t xml:space="preserve">CAMILA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG273</t>
+    <t xml:space="preserve">REG00008</t>
   </si>
   <si>
     <t xml:space="preserve">ROBERTO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG104</t>
+    <t xml:space="preserve">REG00009</t>
   </si>
   <si>
     <t xml:space="preserve">FERNANDA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG672</t>
+    <t xml:space="preserve">REG00010</t>
   </si>
   <si>
     <t xml:space="preserve">ANDRÉ</t>
   </si>
   <si>
-    <t xml:space="preserve">REG835</t>
+    <t xml:space="preserve">REG00011</t>
   </si>
   <si>
     <t xml:space="preserve">LETÍCIA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG329</t>
+    <t xml:space="preserve">REG00012</t>
   </si>
   <si>
     <t xml:space="preserve">BRUNO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG450</t>
+    <t xml:space="preserve">REG00013</t>
   </si>
   <si>
     <t xml:space="preserve">CARLA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG582</t>
+    <t xml:space="preserve">REG00014</t>
   </si>
   <si>
     <t xml:space="preserve">LUCAS</t>
   </si>
   <si>
-    <t xml:space="preserve">REG193</t>
+    <t xml:space="preserve">REG00015</t>
   </si>
   <si>
     <t xml:space="preserve">JULIANA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG405</t>
+    <t xml:space="preserve">REG00016</t>
   </si>
   <si>
     <t xml:space="preserve">MARCOS</t>
   </si>
   <si>
-    <t xml:space="preserve">REG764</t>
+    <t xml:space="preserve">REG00017</t>
   </si>
   <si>
     <t xml:space="preserve">ALICE</t>
   </si>
   <si>
-    <t xml:space="preserve">REG328</t>
+    <t xml:space="preserve">REG00018</t>
   </si>
   <si>
     <t xml:space="preserve">SD</t>
   </si>
   <si>
-    <t xml:space="preserve">REG412</t>
+    <t xml:space="preserve">REG00019</t>
   </si>
   <si>
     <t xml:space="preserve">SOFIA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG713</t>
+    <t xml:space="preserve">REG00020</t>
   </si>
   <si>
     <t xml:space="preserve">HENRIQUE</t>
   </si>
   <si>
-    <t xml:space="preserve">REG418</t>
+    <t xml:space="preserve">REG00021</t>
   </si>
   <si>
     <t xml:space="preserve">PEDRO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG294</t>
+    <t xml:space="preserve">REG00022</t>
   </si>
   <si>
     <t xml:space="preserve">JOANA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG561</t>
+    <t xml:space="preserve">REG00023</t>
   </si>
   <si>
     <t xml:space="preserve">GUSTAVO</t>
   </si>
   <si>
-    <t xml:space="preserve">REG873</t>
+    <t xml:space="preserve">REG00024</t>
   </si>
   <si>
     <t xml:space="preserve">ADRIANA</t>
   </si>
   <si>
-    <t xml:space="preserve">REG690</t>
+    <t xml:space="preserve">REG00025</t>
   </si>
   <si>
     <t xml:space="preserve">FELIPE</t>
@@ -533,7 +533,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,8 +545,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16381" min="16366" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16366" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>